<commit_message>
Completed acceptance criteria 3 for Deliverable 18429
</commit_message>
<xml_diff>
--- a/src/test/resources/datasets/NAMIS-TestFileBase1.xlsx
+++ b/src/test/resources/datasets/NAMIS-TestFileBase1.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="600" windowWidth="24750" windowHeight="9930"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="15405" windowHeight="11085"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -453,7 +454,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -969,7 +970,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1 A2:F11 A12:F25" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F1 A2:F6 A12:F25 A8:F11 B7:F7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>